<commit_message>
updated visualization to plotly and added additional features
</commit_message>
<xml_diff>
--- a/synthetic_graph_data_small.xlsx
+++ b/synthetic_graph_data_small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhooper\Desktop\Data_Science\ISSO\mortal mint\streamlit in analyst desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFBCA8C-84BB-4CF9-A7F9-5B6B7758D208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FB70A1-BF9F-4231-B40A-EA4B88566C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3097" uniqueCount="1355">
   <si>
     <t>address</t>
   </si>
@@ -4095,6 +4095,9 @@
   <si>
     <t>KM6 VIA YUMBO AEROPUERTO ZONA FRANCA DEL PACIFICO B1 MZ L, 
 PALMIRA, VALLE DEL CAUCA, COLOMBIA</t>
+  </si>
+  <si>
+    <t>node</t>
   </si>
 </sst>
 </file>
@@ -4503,8 +4506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EZ434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC57" workbookViewId="0">
-      <selection activeCell="AJ62" sqref="AJ62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.850000000000001" customHeight="1"/>
@@ -5171,6 +5174,9 @@
       <c r="F3" t="s">
         <v>159</v>
       </c>
+      <c r="EP3" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="4" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="A4" t="s">
@@ -5191,6 +5197,9 @@
       <c r="F4" t="s">
         <v>159</v>
       </c>
+      <c r="EP4" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="5" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="A5" t="s">
@@ -5211,6 +5220,9 @@
       <c r="F5" t="s">
         <v>159</v>
       </c>
+      <c r="EP5" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="6" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="A6" t="s">
@@ -5231,6 +5243,9 @@
       <c r="F6" t="s">
         <v>159</v>
       </c>
+      <c r="EP6" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="7" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="A7" t="s">
@@ -5251,6 +5266,9 @@
       <c r="F7" t="s">
         <v>159</v>
       </c>
+      <c r="EP7" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="8" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="A8" t="s">
@@ -5271,6 +5289,9 @@
       <c r="F8" t="s">
         <v>159</v>
       </c>
+      <c r="EP8" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="9" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="A9" t="s">
@@ -5291,6 +5312,9 @@
       <c r="F9" t="s">
         <v>159</v>
       </c>
+      <c r="EP9" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="10" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="A10" t="s">
@@ -5311,6 +5335,9 @@
       <c r="F10" t="s">
         <v>159</v>
       </c>
+      <c r="EP10" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="11" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="A11" t="s">
@@ -5331,6 +5358,9 @@
       <c r="F11" t="s">
         <v>159</v>
       </c>
+      <c r="EP11" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="12" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="A12" t="s">
@@ -5351,6 +5381,9 @@
       <c r="F12" t="s">
         <v>159</v>
       </c>
+      <c r="EP12" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="13" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="B13" t="s">
@@ -5404,6 +5437,9 @@
       <c r="R13">
         <v>277319152</v>
       </c>
+      <c r="EP13" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="14" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="B14" t="s">
@@ -5457,6 +5493,9 @@
       <c r="R14">
         <v>589765523</v>
       </c>
+      <c r="EP14" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="15" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="B15" t="s">
@@ -5510,6 +5549,9 @@
       <c r="R15">
         <v>884270385</v>
       </c>
+      <c r="EP15" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="16" spans="1:156" ht="16.850000000000001" customHeight="1">
       <c r="B16" t="s">
@@ -5563,8 +5605,11 @@
       <c r="R16">
         <v>417941223</v>
       </c>
-    </row>
-    <row r="17" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP16" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="17" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B17" t="s">
         <v>195</v>
       </c>
@@ -5616,8 +5661,11 @@
       <c r="R17">
         <v>498522186</v>
       </c>
-    </row>
-    <row r="18" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP17" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="18" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B18" t="s">
         <v>195</v>
       </c>
@@ -5669,8 +5717,11 @@
       <c r="R18">
         <v>340564868</v>
       </c>
-    </row>
-    <row r="19" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP18" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="19" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B19" t="s">
         <v>195</v>
       </c>
@@ -5722,8 +5773,11 @@
       <c r="R19">
         <v>959311185</v>
       </c>
-    </row>
-    <row r="20" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP19" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="20" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B20" t="s">
         <v>195</v>
       </c>
@@ -5775,8 +5829,11 @@
       <c r="R20">
         <v>331133095</v>
       </c>
-    </row>
-    <row r="21" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP20" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="21" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B21" t="s">
         <v>195</v>
       </c>
@@ -5828,8 +5885,11 @@
       <c r="R21">
         <v>327357330</v>
       </c>
-    </row>
-    <row r="22" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP21" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="22" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B22" t="s">
         <v>195</v>
       </c>
@@ -5881,8 +5941,11 @@
       <c r="R22">
         <v>207873075</v>
       </c>
-    </row>
-    <row r="23" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP22" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="23" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B23" t="s">
         <v>260</v>
       </c>
@@ -5907,8 +5970,11 @@
       <c r="W23" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="24" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP23" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="24" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B24" t="s">
         <v>260</v>
       </c>
@@ -5933,8 +5999,11 @@
       <c r="W24" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="25" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP24" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="25" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B25" t="s">
         <v>260</v>
       </c>
@@ -5959,8 +6028,11 @@
       <c r="W25" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="26" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP25" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="26" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B26" t="s">
         <v>260</v>
       </c>
@@ -5985,8 +6057,11 @@
       <c r="W26" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="27" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP26" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="27" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B27" t="s">
         <v>260</v>
       </c>
@@ -6011,8 +6086,11 @@
       <c r="W27" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="28" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP27" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="28" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B28" t="s">
         <v>260</v>
       </c>
@@ -6037,8 +6115,11 @@
       <c r="W28" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="29" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP28" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="29" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B29" t="s">
         <v>260</v>
       </c>
@@ -6063,8 +6144,11 @@
       <c r="W29" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="30" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP29" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="30" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B30" t="s">
         <v>260</v>
       </c>
@@ -6089,8 +6173,11 @@
       <c r="W30" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="31" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP30" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="31" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B31" t="s">
         <v>260</v>
       </c>
@@ -6115,8 +6202,11 @@
       <c r="W31" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="32" spans="2:23" ht="16.850000000000001" customHeight="1">
+      <c r="EP31" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="32" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B32" t="s">
         <v>260</v>
       </c>
@@ -6141,8 +6231,11 @@
       <c r="W32" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="33" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP32" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="33" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B33" t="s">
         <v>23</v>
       </c>
@@ -6161,8 +6254,11 @@
       <c r="Z33" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="34" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP33" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="34" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B34" t="s">
         <v>23</v>
       </c>
@@ -6181,8 +6277,11 @@
       <c r="Z34" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="35" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP34" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="35" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B35" t="s">
         <v>23</v>
       </c>
@@ -6198,8 +6297,11 @@
       <c r="Z35" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="36" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP35" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="36" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B36" t="s">
         <v>23</v>
       </c>
@@ -6218,8 +6320,11 @@
       <c r="Z36" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="37" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP36" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="37" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B37" t="s">
         <v>23</v>
       </c>
@@ -6235,8 +6340,11 @@
       <c r="Z37" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="38" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP37" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="38" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B38" t="s">
         <v>23</v>
       </c>
@@ -6252,8 +6360,11 @@
       <c r="Z38" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="39" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP38" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="39" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B39" t="s">
         <v>23</v>
       </c>
@@ -6272,8 +6383,11 @@
       <c r="Z39" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="40" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP39" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="40" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B40" t="s">
         <v>23</v>
       </c>
@@ -6292,8 +6406,11 @@
       <c r="Z40" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="41" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP40" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="41" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B41" t="s">
         <v>23</v>
       </c>
@@ -6309,8 +6426,11 @@
       <c r="Z41" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="42" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP41" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="42" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B42" t="s">
         <v>23</v>
       </c>
@@ -6329,8 +6449,11 @@
       <c r="Z42" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="43" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP42" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="43" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A43" t="s">
         <v>356</v>
       </c>
@@ -6361,8 +6484,11 @@
       <c r="AC43" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="44" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP43" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="44" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A44" t="s">
         <v>363</v>
       </c>
@@ -6393,8 +6519,11 @@
       <c r="AC44" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="45" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP44" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="45" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A45" t="s">
         <v>369</v>
       </c>
@@ -6425,8 +6554,11 @@
       <c r="AC45" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="46" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP45" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="46" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A46" t="s">
         <v>375</v>
       </c>
@@ -6457,8 +6589,11 @@
       <c r="AC46" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="47" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP46" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="47" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A47" t="s">
         <v>382</v>
       </c>
@@ -6489,8 +6624,11 @@
       <c r="AC47" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="48" spans="1:29" ht="16.850000000000001" customHeight="1">
+      <c r="EP47" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="48" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A48" t="s">
         <v>387</v>
       </c>
@@ -6521,8 +6659,11 @@
       <c r="AC48" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="49" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP48" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="49" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A49" t="s">
         <v>394</v>
       </c>
@@ -6553,8 +6694,11 @@
       <c r="AC49" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="50" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP49" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="50" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A50" t="s">
         <v>401</v>
       </c>
@@ -6585,8 +6729,11 @@
       <c r="AC50" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="51" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP50" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="51" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A51" t="s">
         <v>408</v>
       </c>
@@ -6617,8 +6764,11 @@
       <c r="AC51" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="52" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP51" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="52" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="A52" t="s">
         <v>414</v>
       </c>
@@ -6649,8 +6799,11 @@
       <c r="AC52" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="53" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP52" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="53" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B53" t="s">
         <v>420</v>
       </c>
@@ -6678,8 +6831,11 @@
       <c r="AH53" s="2">
         <v>43441.3828125</v>
       </c>
-    </row>
-    <row r="54" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP53" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="54" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B54" t="s">
         <v>420</v>
       </c>
@@ -6707,8 +6863,11 @@
       <c r="AH54" s="2">
         <v>33048.993217592593</v>
       </c>
-    </row>
-    <row r="55" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP54" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="55" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B55" t="s">
         <v>420</v>
       </c>
@@ -6736,8 +6895,11 @@
       <c r="AH55" s="2">
         <v>31088.184270833332</v>
       </c>
-    </row>
-    <row r="56" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP55" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="56" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B56" t="s">
         <v>420</v>
       </c>
@@ -6762,8 +6924,11 @@
       <c r="AH56" s="2">
         <v>40770.154814814807</v>
       </c>
-    </row>
-    <row r="57" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP56" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="57" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B57" t="s">
         <v>420</v>
       </c>
@@ -6791,8 +6956,11 @@
       <c r="AH57" s="2">
         <v>29608.90695601852</v>
       </c>
-    </row>
-    <row r="58" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP57" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="58" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B58" t="s">
         <v>420</v>
       </c>
@@ -6820,8 +6988,11 @@
       <c r="AH58" s="2">
         <v>43416.045347222222</v>
       </c>
-    </row>
-    <row r="59" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP58" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="59" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B59" t="s">
         <v>420</v>
       </c>
@@ -6849,8 +7020,11 @@
       <c r="AH59" s="2">
         <v>35548.05269675926</v>
       </c>
-    </row>
-    <row r="60" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP59" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="60" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B60" t="s">
         <v>420</v>
       </c>
@@ -6878,8 +7052,11 @@
       <c r="AH60" s="2">
         <v>32961.821898148148</v>
       </c>
-    </row>
-    <row r="61" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP60" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="61" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B61" t="s">
         <v>420</v>
       </c>
@@ -6907,8 +7084,11 @@
       <c r="AH61" s="2">
         <v>37277.52553240741</v>
       </c>
-    </row>
-    <row r="62" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP61" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="62" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B62" t="s">
         <v>420</v>
       </c>
@@ -6936,8 +7116,11 @@
       <c r="AH62" s="2">
         <v>31255.883263888889</v>
       </c>
-    </row>
-    <row r="63" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP62" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="63" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B63" t="s">
         <v>0</v>
       </c>
@@ -6977,8 +7160,11 @@
       <c r="AO63" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="64" spans="1:41" ht="16.850000000000001" customHeight="1">
+      <c r="EP63" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="64" spans="1:146" ht="16.850000000000001" customHeight="1">
       <c r="B64" t="s">
         <v>0</v>
       </c>
@@ -7018,8 +7204,11 @@
       <c r="AO64" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="65" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP64" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="65" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B65" t="s">
         <v>0</v>
       </c>
@@ -7059,8 +7248,11 @@
       <c r="AO65" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="66" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP65" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="66" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B66" t="s">
         <v>0</v>
       </c>
@@ -7100,8 +7292,11 @@
       <c r="AO66" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="67" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP66" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="67" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B67" t="s">
         <v>0</v>
       </c>
@@ -7141,8 +7336,11 @@
       <c r="AO67" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="68" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP67" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="68" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B68" t="s">
         <v>0</v>
       </c>
@@ -7182,8 +7380,11 @@
       <c r="AO68" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="69" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP68" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="69" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B69" t="s">
         <v>0</v>
       </c>
@@ -7223,8 +7424,11 @@
       <c r="AO69" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="70" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP69" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="70" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B70" t="s">
         <v>0</v>
       </c>
@@ -7264,8 +7468,11 @@
       <c r="AO70" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="71" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP70" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="71" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B71" t="s">
         <v>0</v>
       </c>
@@ -7305,8 +7512,11 @@
       <c r="AO71" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="72" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP71" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="72" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B72" t="s">
         <v>0</v>
       </c>
@@ -7346,8 +7556,11 @@
       <c r="AO72" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="73" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP72" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="73" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B73" t="s">
         <v>41</v>
       </c>
@@ -7366,8 +7579,11 @@
       <c r="AQ73" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="74" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP73" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="74" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B74" t="s">
         <v>41</v>
       </c>
@@ -7383,8 +7599,11 @@
       <c r="AQ74" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="75" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP74" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="75" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B75" t="s">
         <v>41</v>
       </c>
@@ -7400,8 +7619,11 @@
       <c r="AQ75" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="76" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP75" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="76" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B76" t="s">
         <v>41</v>
       </c>
@@ -7417,8 +7639,11 @@
       <c r="AQ76" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="77" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP76" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="77" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B77" t="s">
         <v>41</v>
       </c>
@@ -7434,8 +7659,11 @@
       <c r="AQ77" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="78" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP77" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="78" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B78" t="s">
         <v>41</v>
       </c>
@@ -7451,8 +7679,11 @@
       <c r="AQ78" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="79" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP78" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="79" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B79" t="s">
         <v>41</v>
       </c>
@@ -7468,8 +7699,11 @@
       <c r="AQ79" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="80" spans="2:43" ht="16.850000000000001" customHeight="1">
+      <c r="EP79" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="80" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B80" t="s">
         <v>41</v>
       </c>
@@ -7485,8 +7719,11 @@
       <c r="AQ80" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="81" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP80" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="81" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B81" t="s">
         <v>41</v>
       </c>
@@ -7502,8 +7739,11 @@
       <c r="AQ81" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="82" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP81" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="82" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B82" t="s">
         <v>41</v>
       </c>
@@ -7519,8 +7759,11 @@
       <c r="AQ82" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="83" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP82" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="83" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B83" t="s">
         <v>558</v>
       </c>
@@ -7551,8 +7794,11 @@
       <c r="AX83" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="84" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP83" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="84" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B84" t="s">
         <v>558</v>
       </c>
@@ -7583,8 +7829,11 @@
       <c r="AX84" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="85" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP84" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="85" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B85" t="s">
         <v>558</v>
       </c>
@@ -7615,8 +7864,11 @@
       <c r="AX85" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="86" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP85" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="86" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B86" t="s">
         <v>558</v>
       </c>
@@ -7647,8 +7899,11 @@
       <c r="AX86" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="87" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP86" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="87" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B87" t="s">
         <v>558</v>
       </c>
@@ -7679,8 +7934,11 @@
       <c r="AX87" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="88" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP87" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="88" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B88" t="s">
         <v>558</v>
       </c>
@@ -7711,8 +7969,11 @@
       <c r="AX88" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="89" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP88" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="89" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B89" t="s">
         <v>558</v>
       </c>
@@ -7743,8 +8004,11 @@
       <c r="AX89" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="90" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP89" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="90" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B90" t="s">
         <v>558</v>
       </c>
@@ -7775,8 +8039,11 @@
       <c r="AX90" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="91" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP90" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="91" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B91" t="s">
         <v>558</v>
       </c>
@@ -7807,8 +8074,11 @@
       <c r="AX91" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="92" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP91" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="92" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B92" t="s">
         <v>558</v>
       </c>
@@ -7839,8 +8109,11 @@
       <c r="AX92" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="93" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP92" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="93" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B93" t="s">
         <v>12</v>
       </c>
@@ -7883,8 +8156,11 @@
       <c r="BH93" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="94" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP93" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="94" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B94" t="s">
         <v>12</v>
       </c>
@@ -7927,8 +8203,11 @@
       <c r="BH94" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="95" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP94" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="95" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B95" t="s">
         <v>12</v>
       </c>
@@ -7971,8 +8250,11 @@
       <c r="BH95" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="96" spans="2:60" ht="16.850000000000001" customHeight="1">
+      <c r="EP95" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="96" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B96" t="s">
         <v>12</v>
       </c>
@@ -8015,8 +8297,11 @@
       <c r="BH96" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="97" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP96" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="97" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B97" t="s">
         <v>12</v>
       </c>
@@ -8059,8 +8344,11 @@
       <c r="BH97" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="98" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP97" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="98" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B98" t="s">
         <v>12</v>
       </c>
@@ -8103,8 +8391,11 @@
       <c r="BH98" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="99" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP98" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="99" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B99" t="s">
         <v>12</v>
       </c>
@@ -8147,8 +8438,11 @@
       <c r="BH99" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="100" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP99" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="100" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B100" t="s">
         <v>12</v>
       </c>
@@ -8191,8 +8485,11 @@
       <c r="BH100" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="101" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP100" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="101" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B101" t="s">
         <v>12</v>
       </c>
@@ -8235,8 +8532,11 @@
       <c r="BH101" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="102" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP101" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="102" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B102" t="s">
         <v>12</v>
       </c>
@@ -8279,8 +8579,11 @@
       <c r="BH102" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="103" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP102" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="103" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B103" t="s">
         <v>61</v>
       </c>
@@ -8302,8 +8605,11 @@
       <c r="BK103" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="104" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP103" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="104" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B104" t="s">
         <v>61</v>
       </c>
@@ -8325,8 +8631,11 @@
       <c r="BK104" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="105" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP104" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="105" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B105" t="s">
         <v>61</v>
       </c>
@@ -8348,8 +8657,11 @@
       <c r="BK105" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="106" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP105" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="106" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B106" t="s">
         <v>61</v>
       </c>
@@ -8371,8 +8683,11 @@
       <c r="BK106" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="107" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP106" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="107" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B107" t="s">
         <v>61</v>
       </c>
@@ -8394,8 +8709,11 @@
       <c r="BK107" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="108" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP107" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="108" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B108" t="s">
         <v>61</v>
       </c>
@@ -8417,8 +8735,11 @@
       <c r="BK108" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="109" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP108" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="109" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B109" t="s">
         <v>61</v>
       </c>
@@ -8440,8 +8761,11 @@
       <c r="BK109" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="110" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP109" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="110" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B110" t="s">
         <v>61</v>
       </c>
@@ -8463,8 +8787,11 @@
       <c r="BK110" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="111" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP110" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="111" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B111" t="s">
         <v>61</v>
       </c>
@@ -8486,8 +8813,11 @@
       <c r="BK111" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="112" spans="2:63" ht="16.850000000000001" customHeight="1">
+      <c r="EP111" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="112" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B112" t="s">
         <v>61</v>
       </c>
@@ -8509,8 +8839,11 @@
       <c r="BK112" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="113" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP112" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="113" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B113" t="s">
         <v>713</v>
       </c>
@@ -8532,8 +8865,11 @@
       <c r="BO113">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP113" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="114" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B114" t="s">
         <v>713</v>
       </c>
@@ -8555,8 +8891,11 @@
       <c r="BO114">
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP114" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="115" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B115" t="s">
         <v>713</v>
       </c>
@@ -8578,8 +8917,11 @@
       <c r="BO115">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP115" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="116" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B116" t="s">
         <v>713</v>
       </c>
@@ -8601,8 +8943,11 @@
       <c r="BO116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP116" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="117" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B117" t="s">
         <v>713</v>
       </c>
@@ -8624,8 +8969,11 @@
       <c r="BO117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP117" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="118" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B118" t="s">
         <v>713</v>
       </c>
@@ -8647,8 +8995,11 @@
       <c r="BO118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP118" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="119" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B119" t="s">
         <v>713</v>
       </c>
@@ -8670,8 +9021,11 @@
       <c r="BO119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP119" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="120" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B120" t="s">
         <v>713</v>
       </c>
@@ -8693,8 +9047,11 @@
       <c r="BO120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP120" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="121" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B121" t="s">
         <v>713</v>
       </c>
@@ -8716,8 +9073,11 @@
       <c r="BO121">
         <v>2</v>
       </c>
-    </row>
-    <row r="122" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP121" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="122" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B122" t="s">
         <v>713</v>
       </c>
@@ -8739,8 +9099,11 @@
       <c r="BO122">
         <v>2</v>
       </c>
-    </row>
-    <row r="123" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP122" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="123" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B123" t="s">
         <v>730</v>
       </c>
@@ -8786,8 +9149,11 @@
       <c r="CA123">
         <v>371262508</v>
       </c>
-    </row>
-    <row r="124" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP123" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="124" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B124" t="s">
         <v>730</v>
       </c>
@@ -8833,8 +9199,11 @@
       <c r="CA124">
         <v>465270475</v>
       </c>
-    </row>
-    <row r="125" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP124" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="125" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B125" t="s">
         <v>730</v>
       </c>
@@ -8880,8 +9249,11 @@
       <c r="CA125">
         <v>938849134</v>
       </c>
-    </row>
-    <row r="126" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP125" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="126" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B126" t="s">
         <v>730</v>
       </c>
@@ -8927,8 +9299,11 @@
       <c r="CA126">
         <v>301061452</v>
       </c>
-    </row>
-    <row r="127" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP126" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="127" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B127" t="s">
         <v>730</v>
       </c>
@@ -8974,8 +9349,11 @@
       <c r="CA127">
         <v>881301762</v>
       </c>
-    </row>
-    <row r="128" spans="2:79" ht="16.850000000000001" customHeight="1">
+      <c r="EP127" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="128" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B128" t="s">
         <v>730</v>
       </c>
@@ -9021,8 +9399,11 @@
       <c r="CA128">
         <v>151630412</v>
       </c>
-    </row>
-    <row r="129" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP128" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="129" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B129" t="s">
         <v>730</v>
       </c>
@@ -9068,8 +9449,11 @@
       <c r="CA129">
         <v>321643310</v>
       </c>
-    </row>
-    <row r="130" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP129" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="130" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B130" t="s">
         <v>730</v>
       </c>
@@ -9115,8 +9499,11 @@
       <c r="CA130">
         <v>977825558</v>
       </c>
-    </row>
-    <row r="131" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP130" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="131" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B131" t="s">
         <v>730</v>
       </c>
@@ -9162,8 +9549,11 @@
       <c r="CA131">
         <v>892823397</v>
       </c>
-    </row>
-    <row r="132" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP131" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="132" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B132" t="s">
         <v>730</v>
       </c>
@@ -9209,8 +9599,11 @@
       <c r="CA132">
         <v>691887352</v>
       </c>
-    </row>
-    <row r="133" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP132" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="133" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B133" t="s">
         <v>757</v>
       </c>
@@ -9397,8 +9790,11 @@
       <c r="EH133">
         <v>9875</v>
       </c>
-    </row>
-    <row r="134" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP133" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="134" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B134" t="s">
         <v>757</v>
       </c>
@@ -9585,8 +9981,11 @@
       <c r="EH134">
         <v>8872</v>
       </c>
-    </row>
-    <row r="135" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP134" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="135" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B135" t="s">
         <v>757</v>
       </c>
@@ -9776,8 +10175,11 @@
       <c r="EH135">
         <v>8677</v>
       </c>
-    </row>
-    <row r="136" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP135" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="136" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B136" t="s">
         <v>757</v>
       </c>
@@ -9964,8 +10366,11 @@
       <c r="EH136">
         <v>4033</v>
       </c>
-    </row>
-    <row r="137" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP136" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="137" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B137" t="s">
         <v>757</v>
       </c>
@@ -10152,8 +10557,11 @@
       <c r="EH137">
         <v>9919</v>
       </c>
-    </row>
-    <row r="138" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP137" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="138" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B138" t="s">
         <v>757</v>
       </c>
@@ -10340,8 +10748,11 @@
       <c r="EH138">
         <v>6151</v>
       </c>
-    </row>
-    <row r="139" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP138" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="139" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B139" t="s">
         <v>757</v>
       </c>
@@ -10531,8 +10942,11 @@
       <c r="EH139">
         <v>9241</v>
       </c>
-    </row>
-    <row r="140" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP139" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="140" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B140" t="s">
         <v>757</v>
       </c>
@@ -10722,8 +11136,11 @@
       <c r="EH140">
         <v>1336</v>
       </c>
-    </row>
-    <row r="141" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP140" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="141" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B141" t="s">
         <v>757</v>
       </c>
@@ -10913,8 +11330,11 @@
       <c r="EH141">
         <v>8883</v>
       </c>
-    </row>
-    <row r="142" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP141" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="142" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B142" t="s">
         <v>757</v>
       </c>
@@ -11104,8 +11524,11 @@
       <c r="EH142">
         <v>2273</v>
       </c>
-    </row>
-    <row r="143" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP142" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="143" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B143" t="s">
         <v>1101</v>
       </c>
@@ -11133,8 +11556,11 @@
       <c r="EM143" t="s">
         <v>1107</v>
       </c>
-    </row>
-    <row r="144" spans="2:143" ht="16.850000000000001" customHeight="1">
+      <c r="EP143" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="144" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B144" t="s">
         <v>1101</v>
       </c>
@@ -11161,6 +11587,9 @@
       </c>
       <c r="EM144" t="s">
         <v>1113</v>
+      </c>
+      <c r="EP144" t="s">
+        <v>1354</v>
       </c>
     </row>
     <row r="145" spans="2:146" ht="16.850000000000001" customHeight="1">
@@ -11191,6 +11620,9 @@
       <c r="EM145" t="s">
         <v>1119</v>
       </c>
+      <c r="EP145" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="146" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B146" t="s">
@@ -11220,6 +11652,9 @@
       <c r="EM146" t="s">
         <v>1125</v>
       </c>
+      <c r="EP146" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="147" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B147" t="s">
@@ -11249,6 +11684,9 @@
       <c r="EM147" t="s">
         <v>1131</v>
       </c>
+      <c r="EP147" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="148" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B148" t="s">
@@ -11278,6 +11716,9 @@
       <c r="EM148" t="s">
         <v>1137</v>
       </c>
+      <c r="EP148" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="149" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B149" t="s">
@@ -11307,6 +11748,9 @@
       <c r="EM149" t="s">
         <v>1142</v>
       </c>
+      <c r="EP149" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="150" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B150" t="s">
@@ -11336,6 +11780,9 @@
       <c r="EM150" t="s">
         <v>1148</v>
       </c>
+      <c r="EP150" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="151" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B151" t="s">
@@ -11365,6 +11812,9 @@
       <c r="EM151" t="s">
         <v>1153</v>
       </c>
+      <c r="EP151" t="s">
+        <v>1354</v>
+      </c>
     </row>
     <row r="152" spans="2:146" ht="16.850000000000001" customHeight="1">
       <c r="B152" t="s">
@@ -11393,6 +11843,9 @@
       </c>
       <c r="EM152" t="s">
         <v>1159</v>
+      </c>
+      <c r="EP152" t="s">
+        <v>1354</v>
       </c>
     </row>
     <row r="153" spans="2:146" ht="16.850000000000001" customHeight="1">

</xml_diff>